<commit_message>
Updating the repository for broodjes
Now we have both the spreadsheet and CSV for data processing
</commit_message>
<xml_diff>
--- a/broodjes.xlsx
+++ b/broodjes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dragonbe/workspace/in2it-training/talent-it/lunch-order-app-talent-it-php-class/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4B90E96-2DC1-724B-8035-717DA1C44981}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EBEC61-3632-C44A-B3E2-1EBE1755BF67}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16060" xr2:uid="{1D3A57A1-A9DB-574A-AFD8-FBCC5CB29565}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{1D3A57A1-A9DB-574A-AFD8-FBCC5CB29565}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="115">
   <si>
     <t>Categorie</t>
   </si>
@@ -226,6 +226,150 @@
   </si>
   <si>
     <t>Currydressing, sojascheuten, appel</t>
+  </si>
+  <si>
+    <t>BBQ Chicken</t>
+  </si>
+  <si>
+    <t>Kip, BBQ saus, Bicky ajuin, Cheddar</t>
+  </si>
+  <si>
+    <t>Carpaccio</t>
+  </si>
+  <si>
+    <t>Carpaccio, pesto, pijnboompitten, parmezaan, rucola</t>
+  </si>
+  <si>
+    <t>Bribri</t>
+  </si>
+  <si>
+    <t>Brie, honing, noten</t>
+  </si>
+  <si>
+    <t>Fitness zalm</t>
+  </si>
+  <si>
+    <t>Kruidenkaas, rucola, zalm, ajuin</t>
+  </si>
+  <si>
+    <t>Caesar</t>
+  </si>
+  <si>
+    <t>Kip, Rucola, Caesardressing, spek, parmezaan</t>
+  </si>
+  <si>
+    <t>Nicoise</t>
+  </si>
+  <si>
+    <t>Tonijnsla, sla, tomaat, ansjovis, ajuin, ei</t>
+  </si>
+  <si>
+    <t>Italia</t>
+  </si>
+  <si>
+    <t>Parmaham, pesto, mozzarella, tomaat</t>
+  </si>
+  <si>
+    <t>Zomerbroodje (seizoen)</t>
+  </si>
+  <si>
+    <t>Kip, rucola, bieslookdressing, zongedroogde tomaten</t>
+  </si>
+  <si>
+    <t>Bicky</t>
+  </si>
+  <si>
+    <t>Boulet, Bicky saus, ketchup, Bicky ajuin, augurk</t>
+  </si>
+  <si>
+    <t>Martino Royal</t>
+  </si>
+  <si>
+    <t>Prepare, martinosaus, mosterd, augurk, ajuin, ansjovis</t>
+  </si>
+  <si>
+    <t>Martino Bicky</t>
+  </si>
+  <si>
+    <t>Prepare, Bicky saus, Bicky ajuin, ketchup</t>
+  </si>
+  <si>
+    <t>Geitenkaas</t>
+  </si>
+  <si>
+    <t>Spek, appel, honing, rucola</t>
+  </si>
+  <si>
+    <t>Croques</t>
+  </si>
+  <si>
+    <t>Uit het vuistje</t>
+  </si>
+  <si>
+    <t>Zonder garnituur</t>
+  </si>
+  <si>
+    <t>Croque Monsieur</t>
+  </si>
+  <si>
+    <t>Croque Madame</t>
+  </si>
+  <si>
+    <t>+ spiegelei</t>
+  </si>
+  <si>
+    <t>+ ananas</t>
+  </si>
+  <si>
+    <t>Croque Zalm</t>
+  </si>
+  <si>
+    <t>Brie, spek en honing</t>
+  </si>
+  <si>
+    <t>Panini</t>
+  </si>
+  <si>
+    <t>Mozzarella</t>
+  </si>
+  <si>
+    <t>Tomaat</t>
+  </si>
+  <si>
+    <t>Hawaï</t>
+  </si>
+  <si>
+    <t>Ham, ananas</t>
+  </si>
+  <si>
+    <t>Croque Hawaï</t>
+  </si>
+  <si>
+    <t>Fromaggi</t>
+  </si>
+  <si>
+    <t>Jonge kaas, brie</t>
+  </si>
+  <si>
+    <t>Zalm</t>
+  </si>
+  <si>
+    <t>Gerookte zalm, ajuin</t>
+  </si>
+  <si>
+    <t>Tonijn, ajuin</t>
+  </si>
+  <si>
+    <t>Ham, tomaat</t>
+  </si>
+  <si>
+    <t>Kippewit, tomaat</t>
+  </si>
+  <si>
+    <t>Croque oude leeuw</t>
+  </si>
+  <si>
+    <t>Spek, brie, honing, tomaat</t>
   </si>
 </sst>
 </file>
@@ -261,9 +405,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C989DBC-0DD2-574E-97EE-D62B7ED9FD37}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection sqref="A1:E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1298,6 +1443,9 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>62</v>
+      </c>
       <c r="B50" t="s">
         <v>65</v>
       </c>
@@ -1309,6 +1457,442 @@
       </c>
       <c r="E50" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="D51" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E51" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>62</v>
+      </c>
+      <c r="B52" t="s">
+        <v>69</v>
+      </c>
+      <c r="C52" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="D52" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="E52" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="D53" s="1">
+        <v>3.9</v>
+      </c>
+      <c r="E53" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" t="s">
+        <v>73</v>
+      </c>
+      <c r="C54" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="D54" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E54" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" t="s">
+        <v>75</v>
+      </c>
+      <c r="C55" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="D55" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="E55" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>62</v>
+      </c>
+      <c r="B56" t="s">
+        <v>77</v>
+      </c>
+      <c r="C56" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="D56" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="E56" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" t="s">
+        <v>79</v>
+      </c>
+      <c r="C57" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="D57" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="E57" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58" t="s">
+        <v>81</v>
+      </c>
+      <c r="C58" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="D58" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E58" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="D59" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="E59" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" t="s">
+        <v>85</v>
+      </c>
+      <c r="C60" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="D60" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="E60" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" t="s">
+        <v>87</v>
+      </c>
+      <c r="C61" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="D61" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="E61" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" t="s">
+        <v>89</v>
+      </c>
+      <c r="C62" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="D62" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E62" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>91</v>
+      </c>
+      <c r="B63" t="s">
+        <v>92</v>
+      </c>
+      <c r="C63" s="1">
+        <v>3</v>
+      </c>
+      <c r="D63" s="1">
+        <v>3</v>
+      </c>
+      <c r="E63" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>91</v>
+      </c>
+      <c r="B64" t="s">
+        <v>94</v>
+      </c>
+      <c r="C64" s="1">
+        <v>3.9</v>
+      </c>
+      <c r="D64" s="1">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>91</v>
+      </c>
+      <c r="B65" t="s">
+        <v>95</v>
+      </c>
+      <c r="C65" s="1">
+        <v>5</v>
+      </c>
+      <c r="D65" s="1">
+        <v>5</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>91</v>
+      </c>
+      <c r="B66" t="s">
+        <v>105</v>
+      </c>
+      <c r="C66" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="D66" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>91</v>
+      </c>
+      <c r="B67" t="s">
+        <v>98</v>
+      </c>
+      <c r="C67" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="D67" s="1">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>91</v>
+      </c>
+      <c r="B68" t="s">
+        <v>113</v>
+      </c>
+      <c r="C68" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="D68" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="E68" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>100</v>
+      </c>
+      <c r="B69" t="s">
+        <v>101</v>
+      </c>
+      <c r="C69" s="1">
+        <v>5</v>
+      </c>
+      <c r="D69" s="1">
+        <v>5</v>
+      </c>
+      <c r="E69" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>100</v>
+      </c>
+      <c r="B70" t="s">
+        <v>103</v>
+      </c>
+      <c r="C70" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="D70" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="E70" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>100</v>
+      </c>
+      <c r="B71" t="s">
+        <v>106</v>
+      </c>
+      <c r="C71" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="D71" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="E71" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>100</v>
+      </c>
+      <c r="B72" t="s">
+        <v>108</v>
+      </c>
+      <c r="C72" s="1">
+        <v>6</v>
+      </c>
+      <c r="D72" s="1">
+        <v>6</v>
+      </c>
+      <c r="E72" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>100</v>
+      </c>
+      <c r="B73" t="s">
+        <v>43</v>
+      </c>
+      <c r="C73" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="D73" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="E73" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>100</v>
+      </c>
+      <c r="B74" t="s">
+        <v>13</v>
+      </c>
+      <c r="C74" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="D74" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="E74" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>100</v>
+      </c>
+      <c r="B75" t="s">
+        <v>27</v>
+      </c>
+      <c r="C75" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="D75" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="E75" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>100</v>
+      </c>
+      <c r="B76" t="s">
+        <v>36</v>
+      </c>
+      <c r="C76" s="1">
+        <v>6.9</v>
+      </c>
+      <c r="D76" s="1">
+        <v>6.9</v>
+      </c>
+      <c r="E76" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>